<commit_message>
basic pdf generation + fixed data parsing
</commit_message>
<xml_diff>
--- a/Woda062024.xlsx
+++ b/Woda062024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igi/Desktop/Projects/excelPDF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA9D1B6-7F0A-4521-A198-25857A1C31D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9315202-D537-2C49-BAB4-FD9855753891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD5EEB7A-8104-4FA8-A3F7-3232662F7F0C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{AD5EEB7A-8104-4FA8-A3F7-3232662F7F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Woda 06" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,62 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'9'!$A$1:$H$38</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>ignacy buczek</author>
+  </authors>
+  <commentList>
+    <comment ref="D25" authorId="0" shapeId="0" xr:uid="{65360995-5F94-DC46-A7FB-8EF0E98DFF2A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ignacy buczek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
   <si>
     <t>Rozliczenie lokali za wodę zimną i podgrzanie od 01.06.2024 do 30.06.2024</t>
   </si>
@@ -300,6 +345,12 @@
   </si>
   <si>
     <t>30.06.</t>
+  </si>
+  <si>
+    <t>Maile</t>
+  </si>
+  <si>
+    <t>cos</t>
   </si>
 </sst>
 </file>
@@ -307,12 +358,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;zł&quot;;[Red]\-#,##0.00\ &quot;zł&quot;"/>
-    <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
-    <numFmt numFmtId="166" formatCode="#,##0.000_ ;[Red]\-#,##0.000\ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;zł&quot;;[Red]\-#,##0.00\ &quot;zł&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0.000_ ;[Red]\-#,##0.000\ "/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,6 +512,19 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -586,13 +650,13 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -614,7 +678,7 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -632,44 +696,32 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -678,8 +730,152 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -690,51 +886,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,130 +913,23 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="18" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="18" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="19" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="13" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="15" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="19" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hiperłącze" xfId="2" builtinId="8"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normalny 9" xfId="1" xr:uid="{004D535C-83C6-4877-AF97-855BBCBA29CE}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,9 +1041,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1019,7 +1081,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1125,7 +1187,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1267,7 +1329,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1275,21 +1337,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79406D6C-E6C3-4E29-9900-755B942BAE09}">
-  <dimension ref="A1:W31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" activeCellId="3" sqref="G28 J28 L28 N28"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
     <col min="20" max="20" width="17.33203125" customWidth="1"/>
-    <col min="23" max="23" width="19.77734375" customWidth="1"/>
+    <col min="23" max="23" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1320,21 +1382,21 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="37" t="s">
+      <c r="F2" s="86"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="87"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1347,7 +1409,7 @@
       <c r="T2" s="6"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:23" ht="66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="70" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1408,9 +1470,11 @@
       <c r="T3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:23" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="U3" s="101" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="17">
@@ -1467,1694 +1531,1691 @@
       <c r="T4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="U4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="U4" s="97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="98">
         <v>1</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="21">
         <v>-90.782941976123482</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="22">
         <v>90.75</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="23">
         <v>39.996000000000002</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="23">
         <v>41.371000000000002</v>
       </c>
-      <c r="G5" s="101">
+      <c r="G5" s="84">
         <v>1.375</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H5" s="23">
         <v>26.93</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>27.597000000000001</v>
       </c>
-      <c r="J5" s="101">
+      <c r="J5" s="84">
         <v>0.66700000000000159</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="23">
         <v>2.0420000000000016</v>
       </c>
-      <c r="L5" s="101">
+      <c r="L5" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="23">
         <v>34.638805903501925</v>
       </c>
-      <c r="N5" s="101">
+      <c r="N5" s="84">
         <v>-0.84570716033076399</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="22">
         <v>33.793098743171164</v>
       </c>
-      <c r="P5" s="101">
+      <c r="P5" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q5" s="101">
+      <c r="Q5" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R5" s="25">
+      <c r="R5" s="23">
         <v>12.760253364817043</v>
       </c>
-      <c r="S5" s="24">
+      <c r="S5" s="22">
         <v>50.561557712643122</v>
       </c>
-      <c r="T5" s="23">
+      <c r="T5" s="21">
         <v>-84.387598431937761</v>
       </c>
-      <c r="U5" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="U5" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="98">
         <v>2</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="21">
         <v>-553.49658692533069</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="22">
         <v>553.54000000000008</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="23">
         <v>100.54</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="23">
         <v>103.57899999999999</v>
       </c>
-      <c r="G6" s="101">
+      <c r="G6" s="84">
         <v>3.0389999999999873</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="23">
         <v>17.245999999999999</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <v>17.591999999999999</v>
       </c>
-      <c r="J6" s="101">
+      <c r="J6" s="84">
         <v>0.34600000000000009</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K6" s="23">
         <v>3.3849999999999874</v>
       </c>
-      <c r="L6" s="101">
+      <c r="L6" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M6" s="25">
+      <c r="M6" s="23">
         <v>57.420351607910618</v>
       </c>
-      <c r="N6" s="101">
+      <c r="N6" s="84">
         <v>-1.4019190684229295</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="22">
         <v>56.018432539487691</v>
       </c>
-      <c r="P6" s="101">
+      <c r="P6" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q6" s="101">
+      <c r="Q6" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R6" s="25">
+      <c r="R6" s="23">
         <v>6.6192618654073279</v>
       </c>
-      <c r="S6" s="24">
+      <c r="S6" s="22">
         <v>44.420566213233414</v>
       </c>
-      <c r="T6" s="27">
+      <c r="T6" s="25">
         <v>-100.39558567805172</v>
       </c>
-      <c r="U6" s="26">
-        <v>2.6414127773932705E-8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="U6" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="98">
         <v>3</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="21">
         <v>-277.33146612052542</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="22">
         <v>277.45</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="23">
         <v>157.29599999999999</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>162.78899999999999</v>
       </c>
-      <c r="G7" s="101">
+      <c r="G7" s="84">
         <v>5.492999999999995</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="23">
         <v>122.054</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <v>125.887</v>
       </c>
-      <c r="J7" s="101">
+      <c r="J7" s="84">
         <v>3.8329999999999984</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K7" s="23">
         <v>9.3259999999999934</v>
       </c>
-      <c r="L7" s="101">
+      <c r="L7" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M7" s="25">
+      <c r="M7" s="23">
         <v>158.19858171207562</v>
       </c>
-      <c r="N7" s="101">
+      <c r="N7" s="84">
         <v>-3.8624216343020024</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="22">
         <v>154.33616007777363</v>
       </c>
-      <c r="P7" s="101">
+      <c r="P7" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q7" s="101">
+      <c r="Q7" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R7" s="25">
+      <c r="R7" s="23">
         <v>73.328412514758</v>
       </c>
-      <c r="S7" s="24">
+      <c r="S7" s="22">
         <v>111.12971686258408</v>
       </c>
-      <c r="T7" s="23">
+      <c r="T7" s="21">
         <v>-265.34734306088313</v>
       </c>
-      <c r="U7" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="U7" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="98">
         <v>4</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="21">
         <v>-434.5587453455575</v>
       </c>
-      <c r="D8" s="24">
-        <v>0</v>
-      </c>
-      <c r="E8" s="25">
+      <c r="D8" s="22">
+        <v>0</v>
+      </c>
+      <c r="E8" s="23">
         <v>52.209000000000003</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="23">
         <v>53.359000000000002</v>
       </c>
-      <c r="G8" s="101">
+      <c r="G8" s="84">
         <v>1.1499999999999986</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="23">
         <v>36.036000000000001</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="23">
         <v>36.508000000000003</v>
       </c>
-      <c r="J8" s="101">
+      <c r="J8" s="84">
         <v>0.47200000000000131</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="23">
         <v>1.6219999999999999</v>
       </c>
-      <c r="L8" s="101">
+      <c r="L8" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M8" s="25">
+      <c r="M8" s="23">
         <v>27.514271878295823</v>
       </c>
-      <c r="N8" s="101">
+      <c r="N8" s="84">
         <v>-0.67176151520886263</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="22">
         <v>26.842510363086959</v>
       </c>
-      <c r="P8" s="101">
+      <c r="P8" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q8" s="101">
+      <c r="Q8" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="23">
         <v>9.029744510035453</v>
       </c>
-      <c r="S8" s="24">
+      <c r="S8" s="22">
         <v>46.831048857861532</v>
       </c>
-      <c r="T8" s="23">
+      <c r="T8" s="21">
         <v>-508.23230456650595</v>
       </c>
-      <c r="U8" s="26">
-        <v>-7.9580786405131221E-13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="U8" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="98">
         <v>5</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="21">
         <v>-141.78850332692934</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="22">
         <v>109.15</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="23">
         <v>8.3659999999999997</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="23">
         <v>8.8450000000000006</v>
       </c>
-      <c r="G9" s="101">
+      <c r="G9" s="84">
         <v>0.47900000000000098</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="23">
         <v>7.2759999999999998</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="23">
         <v>7.7789999999999999</v>
       </c>
-      <c r="J9" s="101">
+      <c r="J9" s="84">
         <v>0.50300000000000011</v>
       </c>
-      <c r="K9" s="25">
+      <c r="K9" s="23">
         <v>0.98200000000000109</v>
       </c>
-      <c r="L9" s="101">
+      <c r="L9" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="23">
         <v>16.65783907798183</v>
       </c>
-      <c r="N9" s="101">
+      <c r="N9" s="84">
         <v>-0.40670148454691973</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="22">
         <v>16.251137593434912</v>
       </c>
-      <c r="P9" s="101">
+      <c r="P9" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q9" s="101">
+      <c r="Q9" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R9" s="25">
+      <c r="R9" s="23">
         <v>9.6227997638725018</v>
       </c>
-      <c r="S9" s="24">
+      <c r="S9" s="22">
         <v>47.424104111698583</v>
       </c>
-      <c r="T9" s="23">
+      <c r="T9" s="21">
         <v>-96.313745032062826</v>
       </c>
-      <c r="U9" s="26">
-        <v>3.694822225952521E-13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="U9" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="98">
         <v>6</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="21">
         <v>-458.61646544479231</v>
       </c>
-      <c r="D10" s="24">
-        <v>0</v>
-      </c>
-      <c r="E10" s="25">
+      <c r="D10" s="22">
+        <v>0</v>
+      </c>
+      <c r="E10" s="23">
         <v>48.667000000000002</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="23">
         <v>49.703000000000003</v>
       </c>
-      <c r="G10" s="101">
+      <c r="G10" s="84">
         <v>1.0360000000000014</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="23">
         <v>22.436</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="23">
         <v>22.966000000000001</v>
       </c>
-      <c r="J10" s="101">
+      <c r="J10" s="84">
         <v>0.53000000000000114</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K10" s="23">
         <v>1.5660000000000025</v>
       </c>
-      <c r="L10" s="101">
+      <c r="L10" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="23">
         <v>26.564334008268393</v>
       </c>
-      <c r="N10" s="101">
+      <c r="N10" s="84">
         <v>-0.64856876252594364</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10" s="22">
         <v>25.915765245742449</v>
       </c>
-      <c r="P10" s="101">
+      <c r="P10" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q10" s="101">
+      <c r="Q10" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R10" s="25">
+      <c r="R10" s="23">
         <v>10.139331759149972</v>
       </c>
-      <c r="S10" s="24">
+      <c r="S10" s="22">
         <v>47.940636106976058</v>
       </c>
-      <c r="T10" s="23">
+      <c r="T10" s="21">
         <v>-532.47286679751085</v>
       </c>
-      <c r="U10" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="U10" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="98">
         <v>7</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="21">
         <v>-279.00593225335319</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="22">
         <v>279.01</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="23">
         <v>107.889</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="23">
         <v>111.09399999999999</v>
       </c>
-      <c r="G11" s="101">
+      <c r="G11" s="84">
         <v>3.2049999999999983</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H11" s="23">
         <v>119.622</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="23">
         <v>123.408</v>
       </c>
-      <c r="J11" s="101">
+      <c r="J11" s="84">
         <v>3.7860000000000014</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K11" s="23">
         <v>6.9909999999999997</v>
       </c>
-      <c r="L11" s="101">
+      <c r="L11" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M11" s="25">
+      <c r="M11" s="23">
         <v>118.58956516718008</v>
       </c>
-      <c r="N11" s="101">
+      <c r="N11" s="84">
         <v>-2.8953666786838217</v>
       </c>
-      <c r="O11" s="24">
+      <c r="O11" s="22">
         <v>115.69419848849626</v>
       </c>
-      <c r="P11" s="101">
+      <c r="P11" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q11" s="101">
+      <c r="Q11" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R11" s="25">
+      <c r="R11" s="23">
         <v>72.429264226682506</v>
       </c>
-      <c r="S11" s="24">
+      <c r="S11" s="22">
         <v>110.2305685745086</v>
       </c>
-      <c r="T11" s="23">
+      <c r="T11" s="21">
         <v>-225.92069931635805</v>
       </c>
-      <c r="U11" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="21" t="s">
+      <c r="U11" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="98">
         <v>8</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="21">
         <v>-362.52724726149978</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="22">
         <v>362.46000000000004</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="23">
         <v>151.08600000000001</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="23">
         <v>155.85400000000001</v>
       </c>
-      <c r="G12" s="101">
+      <c r="G12" s="84">
         <v>4.7680000000000007</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H12" s="23">
         <v>89.864000000000004</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="23">
         <v>92.35</v>
       </c>
-      <c r="J12" s="101">
+      <c r="J12" s="84">
         <v>2.48599999999999</v>
       </c>
-      <c r="K12" s="25">
+      <c r="K12" s="23">
         <v>7.2539999999999907</v>
       </c>
-      <c r="L12" s="101">
+      <c r="L12" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="23">
         <v>123.05088052105897</v>
       </c>
-      <c r="N12" s="101">
+      <c r="N12" s="84">
         <v>-3.00428978503396</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="22">
         <v>120.04659073602501</v>
       </c>
-      <c r="P12" s="101">
+      <c r="P12" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q12" s="101">
+      <c r="Q12" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R12" s="25">
+      <c r="R12" s="23">
         <v>47.559205194805045</v>
       </c>
-      <c r="S12" s="24">
+      <c r="S12" s="22">
         <v>85.360509542631121</v>
       </c>
-      <c r="T12" s="23">
+      <c r="T12" s="21">
         <v>-205.47434754015586</v>
       </c>
-      <c r="U12" s="26">
-        <v>2.8421709430404007E-13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
+      <c r="U12" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="98">
         <v>9</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="21">
         <v>-994.00693518822436</v>
       </c>
-      <c r="D13" s="24">
-        <v>0</v>
-      </c>
-      <c r="E13" s="25">
+      <c r="D13" s="22">
+        <v>0</v>
+      </c>
+      <c r="E13" s="23">
         <v>296.83</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="23">
         <v>305.77699999999999</v>
       </c>
-      <c r="G13" s="101">
+      <c r="G13" s="84">
         <v>8.9470000000000027</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="23">
         <v>253.202</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="23">
         <v>260.036</v>
       </c>
-      <c r="J13" s="101">
-        <v>6.8340000000000032</v>
-      </c>
-      <c r="K13" s="25">
+      <c r="J13" s="84">
+        <v>6.8339999999999996</v>
+      </c>
+      <c r="K13" s="23">
         <v>15.781000000000006</v>
       </c>
-      <c r="L13" s="101">
+      <c r="L13" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="23">
         <v>267.69588440899298</v>
       </c>
-      <c r="N13" s="101">
-        <v>-6.5358005373064527</v>
-      </c>
-      <c r="O13" s="24">
+      <c r="N13" s="84">
+        <v>-6.5358005373064501</v>
+      </c>
+      <c r="O13" s="22">
         <v>261.16008387168654</v>
       </c>
-      <c r="P13" s="101">
+      <c r="P13" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q13" s="101">
+      <c r="Q13" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="23">
         <v>130.73998724911471</v>
       </c>
-      <c r="S13" s="24">
+      <c r="S13" s="22">
         <v>168.54129159694079</v>
       </c>
-      <c r="T13" s="23">
+      <c r="T13" s="21">
         <v>-1423.7083106568516</v>
       </c>
-      <c r="U13" s="26">
-        <v>0</v>
-      </c>
-      <c r="W13" s="99" t="s">
+      <c r="U13" s="82" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="21" t="s">
+    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="98">
         <v>10</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="21">
         <v>-239.3151348082958</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="22">
         <v>239.31</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="23">
         <v>148.75</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="23">
         <v>152.577</v>
       </c>
-      <c r="G14" s="101">
+      <c r="G14" s="84">
         <v>3.8269999999999982</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H14" s="23">
         <v>86.606999999999999</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="23">
         <v>88.936000000000007</v>
       </c>
-      <c r="J14" s="101">
+      <c r="J14" s="84">
         <v>2.3290000000000077</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K14" s="23">
         <v>6.1560000000000059</v>
       </c>
-      <c r="L14" s="101">
+      <c r="L14" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M14" s="25">
+      <c r="M14" s="23">
         <v>104.4253129980205</v>
       </c>
-      <c r="N14" s="101">
+      <c r="N14" s="84">
         <v>-2.5495461699295698</v>
       </c>
-      <c r="O14" s="24">
+      <c r="O14" s="22">
         <v>101.87576682809093</v>
       </c>
-      <c r="P14" s="101">
+      <c r="P14" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q14" s="101">
+      <c r="Q14" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R14" s="25">
+      <c r="R14" s="23">
         <v>44.555667296340211</v>
       </c>
-      <c r="S14" s="24">
+      <c r="S14" s="22">
         <v>82.356971644166293</v>
       </c>
-      <c r="T14" s="23">
+      <c r="T14" s="21">
         <v>-184.237873280553</v>
       </c>
-      <c r="U14" s="26">
-        <v>-2.2737367544323206E-13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="U14" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="98">
         <v>11</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="21">
         <v>-203.96357584947188</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="22">
         <v>203.96</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="23">
         <v>158.44399999999999</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="23">
         <v>164.292</v>
       </c>
-      <c r="G15" s="101">
+      <c r="G15" s="84">
         <v>5.8480000000000132</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="23">
         <v>75.603999999999999</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="23">
         <v>77.572000000000003</v>
       </c>
-      <c r="J15" s="101">
+      <c r="J15" s="84">
         <v>1.9680000000000035</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="23">
         <v>7.8160000000000167</v>
       </c>
-      <c r="L15" s="101">
+      <c r="L15" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="23">
         <v>132.58418557383516</v>
       </c>
-      <c r="N15" s="101">
+      <c r="N15" s="84">
         <v>-3.23704562445899</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15" s="22">
         <v>129.34713994937616</v>
       </c>
-      <c r="P15" s="101">
+      <c r="P15" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q15" s="101">
+      <c r="Q15" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="23">
         <v>37.649443211334223</v>
       </c>
-      <c r="S15" s="24">
+      <c r="S15" s="22">
         <v>75.450747559160305</v>
       </c>
-      <c r="T15" s="23">
+      <c r="T15" s="21">
         <v>-204.80146335800833</v>
       </c>
-      <c r="U15" s="26">
-        <v>5.9685589803848416E-13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="U15" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="98">
         <v>12</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="21">
         <v>-1.5631940186722204E-13</v>
       </c>
-      <c r="D16" s="24">
-        <v>0</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="101"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="101"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="24">
-        <v>0</v>
-      </c>
-      <c r="P16" s="101"/>
-      <c r="Q16" s="101"/>
-      <c r="R16" s="25"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="23">
+      <c r="D16" s="22">
+        <v>0</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="84"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="84"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="84"/>
+      <c r="O16" s="22">
+        <v>0</v>
+      </c>
+      <c r="P16" s="84"/>
+      <c r="Q16" s="84"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="21">
         <v>-1.5631940186722204E-13</v>
       </c>
-      <c r="U16" s="26">
-        <v>1.5631940186722204E-13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="U16" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="98">
         <v>12</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="21">
         <v>-181.41082996700146</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="22">
         <v>181.77</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="23">
         <v>179.762</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="23">
         <v>190.226</v>
       </c>
-      <c r="G17" s="101">
+      <c r="G17" s="84">
         <v>10.463999999999999</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="23">
         <v>71.756</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="23">
         <v>73.283000000000001</v>
       </c>
-      <c r="J17" s="101">
+      <c r="J17" s="84">
         <v>1.527000000000001</v>
       </c>
-      <c r="K17" s="25">
+      <c r="K17" s="23">
         <v>11.991</v>
       </c>
-      <c r="L17" s="101">
+      <c r="L17" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="23">
         <v>203.40544641963331</v>
       </c>
-      <c r="N17" s="101">
+      <c r="N17" s="84">
         <v>-4.9661481682302533</v>
       </c>
-      <c r="O17" s="24">
+      <c r="O17" s="22">
         <v>198.43929825140305</v>
       </c>
-      <c r="P17" s="101">
+      <c r="P17" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q17" s="101">
+      <c r="Q17" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R17" s="25">
+      <c r="R17" s="23">
         <v>29.21275395513582</v>
       </c>
-      <c r="S17" s="24">
+      <c r="S17" s="22">
         <v>67.014058302961899</v>
       </c>
-      <c r="T17" s="23">
+      <c r="T17" s="21">
         <v>-265.0941865213664</v>
       </c>
-      <c r="U17" s="26">
-        <v>-1.1368683772161603E-13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="U17" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="98">
         <v>13</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="21">
         <v>-382.10387860789723</v>
       </c>
-      <c r="D18" s="24">
-        <v>0</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D18" s="22">
+        <v>0</v>
+      </c>
+      <c r="E18" s="23">
         <v>213.26300000000001</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="23">
         <v>218.41399999999999</v>
       </c>
-      <c r="G18" s="101">
+      <c r="G18" s="84">
         <v>5.150999999999982</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="23">
         <v>198.03100000000001</v>
       </c>
-      <c r="I18" s="25">
+      <c r="I18" s="23">
         <v>202.10599999999999</v>
       </c>
-      <c r="J18" s="101">
+      <c r="J18" s="84">
         <v>4.0749999999999886</v>
       </c>
-      <c r="K18" s="25">
+      <c r="K18" s="23">
         <v>9.2259999999999707</v>
       </c>
-      <c r="L18" s="101">
+      <c r="L18" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="23">
         <v>156.50226408702619</v>
       </c>
-      <c r="N18" s="101">
+      <c r="N18" s="84">
         <v>-3.821006004511065</v>
       </c>
-      <c r="O18" s="24">
+      <c r="O18" s="22">
         <v>152.68125808251511</v>
       </c>
-      <c r="P18" s="101">
+      <c r="P18" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q18" s="101">
+      <c r="Q18" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R18" s="25">
+      <c r="R18" s="23">
         <v>77.958069657614956</v>
       </c>
-      <c r="S18" s="24">
+      <c r="S18" s="22">
         <v>115.75937400544103</v>
       </c>
-      <c r="T18" s="23">
+      <c r="T18" s="21">
         <v>-650.54451069585343</v>
       </c>
-      <c r="U18" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
+      <c r="U18" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="98">
         <v>14</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="21">
         <v>-410.43468863596098</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="22">
         <v>207.99</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="23">
         <v>129.697</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="23">
         <v>132.84</v>
       </c>
-      <c r="G19" s="101">
+      <c r="G19" s="84">
         <v>3.1430000000000007</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="23">
         <v>110.983</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="23">
         <v>113.81699999999999</v>
       </c>
-      <c r="J19" s="101">
+      <c r="J19" s="84">
         <v>2.833999999999989</v>
       </c>
-      <c r="K19" s="25">
+      <c r="K19" s="23">
         <v>5.9769999999999897</v>
       </c>
-      <c r="L19" s="101">
+      <c r="L19" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="23">
         <v>101.38890444918241</v>
       </c>
-      <c r="N19" s="101">
+      <c r="N19" s="84">
         <v>-2.4754121926038009</v>
       </c>
-      <c r="O19" s="24">
+      <c r="O19" s="22">
         <v>98.913492256578607</v>
       </c>
-      <c r="P19" s="101">
+      <c r="P19" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q19" s="101">
+      <c r="Q19" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R19" s="25">
+      <c r="R19" s="23">
         <v>54.216728689492165</v>
       </c>
-      <c r="S19" s="24">
+      <c r="S19" s="22">
         <v>92.018033037318247</v>
       </c>
-      <c r="T19" s="23">
+      <c r="T19" s="21">
         <v>-393.37621392985784</v>
       </c>
-      <c r="U19" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="21" t="s">
+      <c r="U19" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="98">
         <v>15</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="21">
         <v>-100.21760798791306</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="22">
         <v>100.23</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="23">
         <v>63.715000000000003</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="23">
         <v>65.335999999999999</v>
       </c>
-      <c r="G20" s="101">
+      <c r="G20" s="84">
         <v>1.6209999999999951</v>
       </c>
-      <c r="H20" s="25">
+      <c r="H20" s="23">
         <v>30.759</v>
       </c>
-      <c r="I20" s="25">
+      <c r="I20" s="23">
         <v>31.638999999999999</v>
       </c>
-      <c r="J20" s="101">
+      <c r="J20" s="84">
         <v>0.87999999999999901</v>
       </c>
-      <c r="K20" s="25">
+      <c r="K20" s="23">
         <v>2.5009999999999941</v>
       </c>
-      <c r="L20" s="101">
+      <c r="L20" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="23">
         <v>42.424903802477004</v>
       </c>
-      <c r="N20" s="101">
+      <c r="N20" s="84">
         <v>-1.0358049010711232</v>
       </c>
-      <c r="O20" s="24">
+      <c r="O20" s="22">
         <v>41.38909890140588</v>
       </c>
-      <c r="P20" s="101">
+      <c r="P20" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q20" s="101">
+      <c r="Q20" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R20" s="25">
+      <c r="R20" s="23">
         <v>16.835116883116878</v>
       </c>
-      <c r="S20" s="24">
+      <c r="S20" s="22">
         <v>54.636421230942958</v>
       </c>
-      <c r="T20" s="23">
+      <c r="T20" s="21">
         <v>-96.013128120261882</v>
       </c>
-      <c r="U20" s="26">
-        <v>-2.7000623958883807E-13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="U20" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="98">
         <v>16</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="21">
         <v>-187.96136153570635</v>
       </c>
-      <c r="D21" s="24">
-        <v>0</v>
-      </c>
-      <c r="E21" s="25">
+      <c r="D21" s="22">
+        <v>0</v>
+      </c>
+      <c r="E21" s="23">
         <v>3.431</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="23">
         <v>3.4329999999999998</v>
       </c>
-      <c r="G21" s="101">
+      <c r="G21" s="84">
         <v>1.9999999999997797E-3</v>
       </c>
-      <c r="H21" s="25">
+      <c r="H21" s="23">
         <v>0.63900000000000001</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="23">
         <v>0.63900000000000001</v>
       </c>
-      <c r="J21" s="101">
-        <v>0</v>
-      </c>
-      <c r="K21" s="25">
+      <c r="J21" s="84">
+        <v>0</v>
+      </c>
+      <c r="K21" s="23">
         <v>1.9999999999997797E-3</v>
       </c>
-      <c r="L21" s="101">
+      <c r="L21" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M21" s="25">
+      <c r="M21" s="23">
         <v>3.3926352500977551E-2</v>
       </c>
-      <c r="N21" s="101">
+      <c r="N21" s="84">
         <v>-8.2831259581848168E-4</v>
       </c>
-      <c r="O21" s="24">
+      <c r="O21" s="22">
         <v>3.3098039905159068E-2</v>
       </c>
-      <c r="P21" s="101">
+      <c r="P21" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q21" s="101">
+      <c r="Q21" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R21" s="25">
-        <v>0</v>
-      </c>
-      <c r="S21" s="24">
+      <c r="R21" s="23">
+        <v>0</v>
+      </c>
+      <c r="S21" s="22">
         <v>37.801304347826083</v>
       </c>
-      <c r="T21" s="23">
+      <c r="T21" s="21">
         <v>-225.79576392343759</v>
       </c>
-      <c r="U21" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="21" t="s">
+      <c r="U21" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="98">
         <v>17</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="21">
         <v>-70.490613459112211</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="22">
         <v>37.799999999999997</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="23">
         <v>3.903</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="23">
         <v>3.903</v>
       </c>
-      <c r="G22" s="101">
-        <v>0</v>
-      </c>
-      <c r="H22" s="25">
+      <c r="G22" s="84">
+        <v>0</v>
+      </c>
+      <c r="H22" s="23">
         <v>2.2570000000000001</v>
       </c>
-      <c r="I22" s="25">
+      <c r="I22" s="23">
         <v>2.2570000000000001</v>
       </c>
-      <c r="J22" s="101">
-        <v>0</v>
-      </c>
-      <c r="K22" s="25">
-        <v>0</v>
-      </c>
-      <c r="L22" s="101">
+      <c r="J22" s="84">
+        <v>0</v>
+      </c>
+      <c r="K22" s="23">
+        <v>0</v>
+      </c>
+      <c r="L22" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M22" s="25">
-        <v>0</v>
-      </c>
-      <c r="N22" s="101">
-        <v>0</v>
-      </c>
-      <c r="O22" s="24">
-        <v>0</v>
-      </c>
-      <c r="P22" s="101">
+      <c r="M22" s="23">
+        <v>0</v>
+      </c>
+      <c r="N22" s="84">
+        <v>0</v>
+      </c>
+      <c r="O22" s="22">
+        <v>0</v>
+      </c>
+      <c r="P22" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q22" s="101">
+      <c r="Q22" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R22" s="25">
-        <v>0</v>
-      </c>
-      <c r="S22" s="24">
+      <c r="R22" s="23">
+        <v>0</v>
+      </c>
+      <c r="S22" s="22">
         <v>37.801304347826083</v>
       </c>
-      <c r="T22" s="23">
+      <c r="T22" s="21">
         <v>-70.491917806938289</v>
       </c>
-      <c r="U22" s="26">
-        <v>-4.6895820560166612E-13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
+      <c r="U22" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="98">
         <v>18</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="21">
         <v>-41.22597316075958</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="22">
         <v>41.32</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="23">
         <v>3.3260000000000001</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="23">
         <v>3.8759999999999999</v>
       </c>
-      <c r="G23" s="101">
+      <c r="G23" s="84">
         <v>0.54999999999999982</v>
       </c>
-      <c r="H23" s="25">
+      <c r="H23" s="23">
         <v>2.2320000000000002</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="23">
         <v>2.5979999999999999</v>
       </c>
-      <c r="J23" s="101">
+      <c r="J23" s="84">
         <v>0.36599999999999966</v>
       </c>
-      <c r="K23" s="25">
+      <c r="K23" s="23">
         <v>0.91599999999999948</v>
       </c>
-      <c r="L23" s="101">
+      <c r="L23" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M23" s="25">
+      <c r="M23" s="23">
         <v>15.538269445449421</v>
       </c>
-      <c r="N23" s="101">
+      <c r="N23" s="84">
         <v>-0.37936716888490618</v>
       </c>
-      <c r="O23" s="24">
+      <c r="O23" s="22">
         <v>15.158902276564515</v>
       </c>
-      <c r="P23" s="101">
+      <c r="P23" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q23" s="101">
+      <c r="Q23" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R23" s="25">
+      <c r="R23" s="23">
         <v>7.0018781582054306</v>
       </c>
-      <c r="S23" s="24">
+      <c r="S23" s="22">
         <v>44.803182506031511</v>
       </c>
-      <c r="T23" s="23">
+      <c r="T23" s="21">
         <v>-59.868057943355609</v>
       </c>
-      <c r="U23" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="21" t="s">
+      <c r="U23" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="98">
         <v>19</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="21">
         <v>-458.70271457525598</v>
       </c>
-      <c r="D24" s="24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="D24" s="22">
+        <v>0</v>
+      </c>
+      <c r="E24" s="23">
         <v>41.737000000000002</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="23">
         <v>42.603000000000002</v>
       </c>
-      <c r="G24" s="101">
+      <c r="G24" s="84">
         <v>0.86599999999999966</v>
       </c>
-      <c r="H24" s="25">
+      <c r="H24" s="23">
         <v>31.492999999999999</v>
       </c>
-      <c r="I24" s="25">
+      <c r="I24" s="23">
         <v>32.232999999999997</v>
       </c>
-      <c r="J24" s="101">
+      <c r="J24" s="84">
         <v>0.73999999999999844</v>
       </c>
-      <c r="K24" s="25">
+      <c r="K24" s="23">
         <v>1.6059999999999981</v>
       </c>
-      <c r="L24" s="101">
+      <c r="L24" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M24" s="25">
+      <c r="M24" s="23">
         <v>27.242861058287943</v>
       </c>
-      <c r="N24" s="101">
+      <c r="N24" s="84">
         <v>-0.66513501444231327</v>
       </c>
-      <c r="O24" s="24">
+      <c r="O24" s="22">
         <v>26.57772604384563</v>
       </c>
-      <c r="P24" s="101">
+      <c r="P24" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q24" s="101">
+      <c r="Q24" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R24" s="25">
+      <c r="R24" s="23">
         <v>14.156802833530088</v>
       </c>
-      <c r="S24" s="24">
+      <c r="S24" s="22">
         <v>51.958107181356169</v>
       </c>
-      <c r="T24" s="23">
+      <c r="T24" s="21">
         <v>-537.23854780045781</v>
       </c>
-      <c r="U24" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="U24" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="98">
         <v>20</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="21">
         <v>-179.60661397456838</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="22">
         <v>179.6</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="23">
         <v>222.41900000000001</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="23">
         <v>229.648</v>
       </c>
-      <c r="G25" s="101">
+      <c r="G25" s="84">
         <v>7.228999999999985</v>
       </c>
-      <c r="H25" s="25">
+      <c r="H25" s="23">
         <v>93.117999999999995</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="23">
         <v>94.972999999999999</v>
       </c>
-      <c r="J25" s="101">
+      <c r="J25" s="84">
         <v>1.855000000000004</v>
       </c>
-      <c r="K25" s="25">
+      <c r="K25" s="23">
         <v>9.083999999999989</v>
       </c>
-      <c r="L25" s="101">
+      <c r="L25" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M25" s="25">
+      <c r="M25" s="23">
         <v>154.09349305945682</v>
       </c>
-      <c r="N25" s="101">
+      <c r="N25" s="84">
         <v>-3.7621958102079534</v>
       </c>
-      <c r="O25" s="24">
+      <c r="O25" s="22">
         <v>150.33129724924888</v>
       </c>
-      <c r="P25" s="101">
+      <c r="P25" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q25" s="101">
+      <c r="Q25" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R25" s="23">
         <v>35.487661157024903</v>
       </c>
-      <c r="S25" s="24">
+      <c r="S25" s="22">
         <v>73.288965504850978</v>
       </c>
-      <c r="T25" s="23">
+      <c r="T25" s="21">
         <v>-223.62687672866824</v>
       </c>
-      <c r="U25" s="26">
-        <v>-4.5474735088646412E-13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="21" t="s">
+      <c r="U25" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="98">
         <v>21</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="21">
         <v>-188.20469376336328</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="22">
         <v>188.31</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="23">
         <v>166.11799999999999</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="23">
         <v>171.03899999999999</v>
       </c>
-      <c r="G26" s="101">
+      <c r="G26" s="84">
         <v>4.9209999999999923</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="23">
         <v>97.62</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="23">
         <v>100.181</v>
       </c>
-      <c r="J26" s="101">
+      <c r="J26" s="84">
         <v>2.5609999999999928</v>
       </c>
-      <c r="K26" s="25">
+      <c r="K26" s="23">
         <v>7.4819999999999851</v>
       </c>
-      <c r="L26" s="101">
+      <c r="L26" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M26" s="25">
+      <c r="M26" s="23">
         <v>126.91848470617074</v>
       </c>
-      <c r="N26" s="101">
+      <c r="N26" s="84">
         <v>-3.098717420957275</v>
       </c>
-      <c r="O26" s="24">
+      <c r="O26" s="22">
         <v>123.81976728521347</v>
       </c>
-      <c r="P26" s="101">
+      <c r="P26" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q26" s="101">
+      <c r="Q26" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R26" s="25">
+      <c r="R26" s="23">
         <v>48.994016292798015</v>
       </c>
-      <c r="S26" s="24">
+      <c r="S26" s="22">
         <v>86.795320640624098</v>
       </c>
-      <c r="T26" s="23">
+      <c r="T26" s="21">
         <v>-210.50978168920085</v>
       </c>
-      <c r="U26" s="26">
-        <v>-2.8421709430404007E-13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="21" t="s">
+      <c r="U26" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="98">
         <v>22</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="21">
         <v>-221.32069638423988</v>
       </c>
-      <c r="D27" s="24">
-        <v>0</v>
-      </c>
-      <c r="E27" s="25">
+      <c r="D27" s="22">
+        <v>0</v>
+      </c>
+      <c r="E27" s="23">
         <v>159.422</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="23">
         <v>165.512</v>
       </c>
-      <c r="G27" s="101">
+      <c r="G27" s="84">
         <v>6.0900000000000034</v>
       </c>
-      <c r="H27" s="25">
+      <c r="H27" s="23">
         <v>97.542000000000002</v>
       </c>
-      <c r="I27" s="25">
+      <c r="I27" s="23">
         <v>101.131</v>
       </c>
-      <c r="J27" s="101">
+      <c r="J27" s="84">
         <v>3.5889999999999986</v>
       </c>
-      <c r="K27" s="25">
+      <c r="K27" s="23">
         <v>9.679000000000002</v>
       </c>
-      <c r="L27" s="101">
+      <c r="L27" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M27" s="25">
+      <c r="M27" s="23">
         <v>164.18658292849898</v>
       </c>
-      <c r="N27" s="101">
+      <c r="N27" s="84">
         <v>-4.0086188074639848</v>
       </c>
-      <c r="O27" s="24">
+      <c r="O27" s="22">
         <v>160.17796412103499</v>
       </c>
-      <c r="P27" s="101">
+      <c r="P27" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q27" s="101">
+      <c r="Q27" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R27" s="25">
+      <c r="R27" s="23">
         <v>68.660493742621043</v>
       </c>
-      <c r="S27" s="24">
+      <c r="S27" s="22">
         <v>106.46179809044713</v>
       </c>
-      <c r="T27" s="23">
+      <c r="T27" s="21">
         <v>-487.960458595722</v>
       </c>
-      <c r="U27" s="26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+      <c r="U27" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="98">
         <v>23</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="26">
         <v>-68.299507526573535</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="22">
         <v>68.34</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="22">
         <v>75.406999999999996</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="22">
         <v>76.807000000000002</v>
       </c>
-      <c r="G28" s="101">
+      <c r="G28" s="84">
         <v>1.4000000000000057</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="22">
         <v>6.8049999999999997</v>
       </c>
-      <c r="I28" s="24">
+      <c r="I28" s="22">
         <v>6.9740000000000002</v>
       </c>
-      <c r="J28" s="101">
+      <c r="J28" s="84">
         <v>0.16900000000000048</v>
       </c>
-      <c r="K28" s="24">
+      <c r="K28" s="22">
         <v>1.5690000000000062</v>
       </c>
-      <c r="L28" s="101">
+      <c r="L28" s="84">
         <v>16.963176250490644</v>
       </c>
-      <c r="M28" s="24">
+      <c r="M28" s="22">
         <v>26.615223537019926</v>
       </c>
-      <c r="N28" s="101">
+      <c r="N28" s="84">
         <v>-0.64981123141967301</v>
       </c>
-      <c r="O28" s="24">
+      <c r="O28" s="22">
         <v>25.965412305600253</v>
       </c>
-      <c r="P28" s="101">
+      <c r="P28" s="84">
         <v>37.801304347826083</v>
       </c>
-      <c r="Q28" s="101">
+      <c r="Q28" s="84">
         <v>19.130814639905566</v>
       </c>
-      <c r="R28" s="24">
+      <c r="R28" s="22">
         <v>3.2331076741440499</v>
       </c>
-      <c r="S28" s="24">
+      <c r="S28" s="22">
         <v>41.034412021970134</v>
       </c>
-      <c r="T28" s="30">
+      <c r="T28" s="26">
         <v>-66.959331854143926</v>
       </c>
-      <c r="U28" s="26">
-        <v>-1.7053025658242404E-13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U28" s="82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="6">
         <v>-6525.372714078454</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="27">
         <v>3120.9900000000007</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="28">
         <v>2532.2729999999997</v>
       </c>
-      <c r="F29" s="32">
+      <c r="F29" s="28">
         <v>2612.877</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="27">
         <v>80.603999999999957</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="28">
         <v>1600.1119999999999</v>
       </c>
-      <c r="I29" s="32">
+      <c r="I29" s="28">
         <v>1642.4619999999998</v>
       </c>
-      <c r="J29" s="31">
+      <c r="J29" s="27">
         <v>42.349999999999966</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="27">
         <v>122.95399999999992</v>
       </c>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32">
+      <c r="L29" s="28"/>
+      <c r="M29" s="28">
         <v>2085.6903727028257</v>
       </c>
-      <c r="N29" s="32">
+      <c r="N29" s="28">
         <v>-50.922173453138377</v>
       </c>
-      <c r="O29" s="31">
+      <c r="O29" s="27">
         <v>2034.7681992496871</v>
       </c>
-      <c r="P29" s="32">
+      <c r="P29" s="28">
         <v>869.43</v>
       </c>
-      <c r="Q29" s="33"/>
-      <c r="R29" s="32">
+      <c r="Q29" s="29"/>
+      <c r="R29" s="28">
         <v>810.1900000000004</v>
       </c>
-      <c r="S29" s="31">
+      <c r="S29" s="27">
         <v>1679.6200000000003</v>
       </c>
-      <c r="T29" s="31">
+      <c r="T29" s="27">
         <v>-7118.7709133281442</v>
       </c>
-      <c r="U29" s="26">
-        <v>2.6412749321025331E-8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U29" s="24"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
         <v>-6525.372714078454</v>
       </c>
-      <c r="D30" s="32">
+      <c r="D30" s="28">
         <v>3120.9900000000007</v>
       </c>
-      <c r="E30" s="32">
+      <c r="E30" s="28">
         <v>2532.2729999999997</v>
       </c>
-      <c r="F30" s="32">
+      <c r="F30" s="28">
         <v>2612.877</v>
       </c>
-      <c r="G30" s="32">
+      <c r="G30" s="28">
         <v>80.603999999999957</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="28">
         <v>1600.1119999999999</v>
       </c>
-      <c r="I30" s="32">
+      <c r="I30" s="28">
         <v>1642.4619999999998</v>
       </c>
-      <c r="J30" s="34">
+      <c r="J30" s="30">
         <v>42.349999999999966</v>
       </c>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="36">
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="32">
         <v>221.53716255849622</v>
       </c>
-      <c r="N30" s="32">
+      <c r="N30" s="28">
         <v>-50.922173453138385</v>
       </c>
-      <c r="O30" s="32">
+      <c r="O30" s="28">
         <v>2034.7681992496871</v>
       </c>
-      <c r="P30" s="32">
+      <c r="P30" s="28">
         <v>869.43</v>
       </c>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="32">
+      <c r="Q30" s="31"/>
+      <c r="R30" s="28">
         <v>810.1900000000004</v>
       </c>
-      <c r="S30" s="24">
+      <c r="S30" s="22">
         <v>1679.6200000000003</v>
       </c>
-      <c r="T30" s="24">
+      <c r="T30" s="22">
         <v>7118.7709133017297</v>
       </c>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="6">
         <v>0</v>
       </c>
-      <c r="D31" s="36">
-        <v>0</v>
-      </c>
-      <c r="E31" s="36">
-        <v>0</v>
-      </c>
-      <c r="F31" s="36">
-        <v>0</v>
-      </c>
-      <c r="G31" s="36">
-        <v>0</v>
-      </c>
-      <c r="H31" s="36">
-        <v>0</v>
-      </c>
-      <c r="I31" s="36">
-        <v>0</v>
-      </c>
-      <c r="J31" s="36">
-        <v>0</v>
-      </c>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="36">
-        <v>0</v>
-      </c>
-      <c r="O31" s="36">
-        <v>0</v>
-      </c>
-      <c r="P31" s="36">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="36">
+      <c r="D31" s="32">
+        <v>0</v>
+      </c>
+      <c r="E31" s="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>0</v>
+      </c>
+      <c r="G31" s="32">
+        <v>0</v>
+      </c>
+      <c r="H31" s="32">
+        <v>0</v>
+      </c>
+      <c r="I31" s="32">
+        <v>0</v>
+      </c>
+      <c r="J31" s="32">
+        <v>0</v>
+      </c>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="32">
+        <v>0</v>
+      </c>
+      <c r="O31" s="32">
+        <v>0</v>
+      </c>
+      <c r="P31" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="32">
         <v>0</v>
       </c>
       <c r="S31" s="6">
@@ -3163,9 +3224,7 @@
       <c r="T31" s="6">
         <v>-2.6414454623591155E-8</v>
       </c>
-      <c r="U31" s="6">
-        <v>-1.7053025658242404E-12</v>
-      </c>
+      <c r="U31" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3173,603 +3232,604 @@
     <mergeCell ref="H2:J2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="W13" r:id="rId1" xr:uid="{F1001CC2-9FA7-4C70-BD62-2A74A66C6263}"/>
+    <hyperlink ref="U5" r:id="rId1" xr:uid="{F1001CC2-9FA7-4C70-BD62-2A74A66C6263}"/>
+    <hyperlink ref="U6:U28" r:id="rId2" display="rafal-buczek@wp.pl" xr:uid="{1E223385-4604-C548-A4A6-B1BEF89F8A2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6372EAB-4537-4F38-A539-301284D7CE37}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6372EAB-4537-4F38-A539-301284D7CE37}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="107" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" style="86" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="3" max="3" width="7.5" style="70" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="44" customWidth="1"/>
+    <col min="8" max="8" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="J1" s="42">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="J1" s="35">
         <f>J36</f>
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="43" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="33"/>
+      <c r="B2" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="40"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="45" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="33"/>
+      <c r="B5" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="40"/>
-      <c r="B7" s="46" t="s">
+      <c r="C5" s="34"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+    </row>
+    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="40"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-    </row>
-    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
-      <c r="B9" s="47" t="s">
+      <c r="C7" s="91"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="33"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="48">
+      <c r="C9" s="39">
         <f>'[1]Kartoteka mieszkanców'!B16</f>
         <v>9</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="40">
         <f>'[1]Kartoteka mieszkanców'!F16</f>
         <v>147.99</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="J11" s="50" t="s">
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="J11" s="41" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="40"/>
-      <c r="J12" s="56"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="J13" s="50"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
-      <c r="B14" s="57" t="s">
+    <row r="12" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="33"/>
+      <c r="J12" s="45"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="J13" s="41"/>
+    </row>
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="33"/>
+      <c r="B14" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="40"/>
-      <c r="J14" s="50"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="J15" s="50"/>
-    </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="63" t="s">
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="33"/>
+      <c r="J14" s="41"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="J15" s="41"/>
+    </row>
+    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="33"/>
+      <c r="B16" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="50"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="41"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:10" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="65" t="s">
+    <row r="17" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="33"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="66" t="s">
+      <c r="F17" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="50"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="41"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="67" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="33"/>
+      <c r="B18" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="69">
+      <c r="D18" s="55">
         <f>'Woda 06'!G13</f>
         <v>8.9470000000000027</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="56">
         <f>'Woda 06'!L5</f>
         <v>16.963176250490644</v>
       </c>
-      <c r="F18" s="71">
+      <c r="F18" s="57">
         <f>E18*D18</f>
         <v>151.76953791313983</v>
       </c>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="56"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="45"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="72" t="s">
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="33"/>
+      <c r="B19" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="69">
+      <c r="D19" s="55">
         <f>'Woda 06'!J13</f>
-        <v>6.8340000000000032</v>
-      </c>
-      <c r="E19" s="70">
+        <v>6.8339999999999996</v>
+      </c>
+      <c r="E19" s="56">
         <f>E18</f>
         <v>16.963176250490644</v>
       </c>
-      <c r="F19" s="71">
+      <c r="F19" s="57">
         <f>E19*D19</f>
-        <v>115.92634649585311</v>
-      </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="56"/>
+        <v>115.92634649585305</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="45"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="72" t="s">
+    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="33"/>
+      <c r="B20" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="69"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="74">
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="60">
         <f>'Woda 06'!N13</f>
-        <v>-6.5358005373064527</v>
-      </c>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="88">
+        <v>-6.5358005373064501</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="72">
         <f>F20-'Woda 06'!N13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="64" t="s">
+    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="33"/>
+      <c r="B21" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="87">
+      <c r="D21" s="71">
         <f>SUM(D18:D20)</f>
-        <v>15.781000000000006</v>
-      </c>
-      <c r="E21" s="74">
+        <v>15.781000000000002</v>
+      </c>
+      <c r="E21" s="60">
         <f>E19</f>
         <v>16.963176250490644</v>
       </c>
-      <c r="F21" s="74">
+      <c r="F21" s="60">
         <f>SUM(F18:F20)</f>
-        <v>261.16008387168648</v>
-      </c>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="88">
+        <v>261.16008387168642</v>
+      </c>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="72">
         <f>F21-'Woda 06'!O13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="40"/>
-      <c r="J22" s="50"/>
-    </row>
-    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="40"/>
-      <c r="B23" s="63" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="33"/>
+      <c r="J22" s="41"/>
+    </row>
+    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="33"/>
+      <c r="B23" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63" t="s">
+      <c r="C23" s="49"/>
+      <c r="D23" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="93" t="s">
+      <c r="E23" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="75" t="s">
+      <c r="F23" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="40"/>
-      <c r="I23" s="50"/>
+      <c r="G23" s="33"/>
+      <c r="I23" s="41"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="65" t="s">
+    <row r="24" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="33"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="89" t="s">
+      <c r="E24" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="66" t="s">
+      <c r="F24" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="G24" s="40"/>
-      <c r="I24" s="50"/>
+      <c r="G24" s="33"/>
+      <c r="I24" s="41"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="40"/>
-      <c r="B25" s="91" t="s">
+    <row r="25" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="33"/>
+      <c r="B25" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="91" t="s">
+      <c r="C25" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="96">
+      <c r="D25" s="79">
         <f>D19</f>
-        <v>6.8340000000000032</v>
-      </c>
-      <c r="E25" s="97">
+        <v>6.8339999999999996</v>
+      </c>
+      <c r="E25" s="80">
         <f>'Woda 06'!Q13</f>
         <v>19.130814639905566</v>
       </c>
-      <c r="F25" s="94">
+      <c r="F25" s="77">
         <f>E25*D25</f>
-        <v>130.73998724911471</v>
-      </c>
-      <c r="G25" s="40"/>
-      <c r="I25" s="50"/>
+        <v>130.73998724911462</v>
+      </c>
+      <c r="G25" s="33"/>
+      <c r="I25" s="41"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="40"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="40"/>
-      <c r="I26" s="50"/>
+    <row r="26" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="33"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="33"/>
+      <c r="I26" s="41"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="93" t="s">
+    <row r="27" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="33"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="75" t="s">
+      <c r="F27" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="40"/>
-      <c r="I27" s="50"/>
+      <c r="G27" s="33"/>
+      <c r="I27" s="41"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="40"/>
-      <c r="B28" s="91" t="s">
+    <row r="28" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="33"/>
+      <c r="B28" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="92">
+      <c r="D28" s="75">
         <f>'Woda 06'!P13</f>
         <v>37.801304347826083</v>
       </c>
-      <c r="E28" s="90">
+      <c r="E28" s="74">
         <v>1</v>
       </c>
-      <c r="F28" s="94">
+      <c r="F28" s="77">
         <f>E28*D28</f>
         <v>37.801304347826083</v>
       </c>
-      <c r="G28" s="40"/>
-      <c r="I28" s="50"/>
+      <c r="G28" s="33"/>
+      <c r="I28" s="41"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="40"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="40"/>
-      <c r="I29" s="50"/>
+    <row r="29" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="33"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="33"/>
+      <c r="I29" s="41"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="40"/>
-      <c r="I30" s="50"/>
+    <row r="30" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="33"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="33"/>
+      <c r="I30" s="41"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="40"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="65"/>
-      <c r="E31" s="90"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="40"/>
-      <c r="I31" s="50"/>
+    <row r="31" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="33"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="33"/>
+      <c r="I31" s="41"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="40"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="I32" s="50"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="I32" s="41"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="40"/>
-      <c r="B33" s="77" t="s">
+    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="33"/>
+      <c r="B33" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="78" t="s">
+      <c r="C33" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="80"/>
-      <c r="F33" s="81">
+      <c r="D33" s="65"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67">
         <f>F25+F28</f>
-        <v>168.54129159694079</v>
-      </c>
-      <c r="G33" s="40"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="88">
+        <v>168.54129159694071</v>
+      </c>
+      <c r="G33" s="33"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="72">
         <f>'Woda 06'!S13-F33</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
-      <c r="B34" s="40"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="I34" s="50"/>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="I34" s="41"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="40"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="J35" s="50"/>
-    </row>
-    <row r="36" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="40"/>
-      <c r="B36" s="82" t="str">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="J35" s="41"/>
+    </row>
+    <row r="36" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="33"/>
+      <c r="B36" s="88" t="str">
         <f>CONCATENATE("Saldo na dzień ",ster!B3,ster!B2,":","                                                                                        [7]+[4]")</f>
         <v>Saldo na dzień 30.06.2024:                                                                                        [7]+[4]</v>
       </c>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="84"/>
-      <c r="F36" s="98">
+      <c r="C36" s="89"/>
+      <c r="D36" s="89"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="81">
         <f>F33+F21</f>
-        <v>429.70137546862725</v>
-      </c>
-      <c r="G36" s="85"/>
-      <c r="H36" s="40"/>
-      <c r="J36" s="56">
+        <v>429.70137546862713</v>
+      </c>
+      <c r="G36" s="69"/>
+      <c r="H36" s="33"/>
+      <c r="J36" s="45">
         <f>F36-'Woda 06'!O13-'Woda 06'!S13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
+    <row r="37" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3784,6 +3844,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3795,9 +3856,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -3805,11 +3866,11 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="83" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
poprawki i inne nie pamietam
</commit_message>
<xml_diff>
--- a/Woda062024.xlsx
+++ b/Woda062024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igi/Desktop/Projects/excelPDF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142B7453-CECE-9B48-AEF4-CE6610C2C191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0AD221-3518-094A-A904-37BC900DD382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{AD5EEB7A-8104-4FA8-A3F7-3232662F7F0C}"/>
   </bookViews>
@@ -643,7 +643,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -890,6 +890,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1340,7 +1341,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+      <selection activeCell="U5" sqref="U5:U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1387,16 +1388,16 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="90" t="s">
+      <c r="E2" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="91"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="90" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="93"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -3233,7 +3234,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="U5" r:id="rId1" xr:uid="{66964BE2-E2AC-BD49-978F-2DDE56A93BCE}"/>
-    <hyperlink ref="U6:U28" r:id="rId2" display="wertex3233@gmail.com" xr:uid="{2643E62E-F319-E640-A6F6-AFD840B08913}"/>
+    <hyperlink ref="U6:U28" r:id="rId2" display="wertex3233@gmail.com" xr:uid="{0BA26D29-335B-2648-8D9E-416C90C8FF33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3244,10 +3245,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="107" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:D36"/>
+    <sheetView topLeftCell="A11" zoomScale="107" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3279,14 +3280,14 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -3337,14 +3338,14 @@
     </row>
     <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="97" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
       <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -3402,9 +3403,9 @@
     </row>
     <row r="12" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="33"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
       <c r="E12" s="42"/>
       <c r="F12" s="43"/>
       <c r="G12" s="44"/>
@@ -3424,14 +3425,14 @@
     </row>
     <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="33"/>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="100"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="101"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="102"/>
       <c r="H14" s="33"/>
       <c r="J14" s="41"/>
     </row>
@@ -3466,7 +3467,7 @@
       <c r="I16" s="41"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33"/>
       <c r="B17" s="48"/>
       <c r="C17" s="49"/>
@@ -3484,7 +3485,7 @@
       <c r="I17" s="41"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="33"/>
       <c r="B18" s="53" t="s">
         <v>75</v>
@@ -3508,8 +3509,20 @@
       <c r="H18" s="33"/>
       <c r="I18" s="45"/>
       <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K18" s="90">
+        <f>ROUND(D18,2)</f>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="L18" s="90">
+        <f>ROUND(E18,2)</f>
+        <v>16.96</v>
+      </c>
+      <c r="M18">
+        <f>ROUND(K18*L18,2)</f>
+        <v>151.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="33"/>
       <c r="B19" s="58" t="s">
         <v>76</v>
@@ -3534,7 +3547,7 @@
       <c r="I19" s="45"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="33"/>
       <c r="B20" s="58" t="s">
         <v>79</v>
@@ -3556,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="33"/>
       <c r="B21" s="50" t="s">
         <v>67</v>
@@ -3584,7 +3597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="33"/>
       <c r="B22" s="33"/>
       <c r="C22" s="46"/>
@@ -3595,7 +3608,7 @@
       <c r="H22" s="33"/>
       <c r="J22" s="41"/>
     </row>
-    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="33"/>
       <c r="B23" s="49" t="s">
         <v>81</v>
@@ -3614,7 +3627,7 @@
       <c r="I23" s="41"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="33"/>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -3631,7 +3644,7 @@
       <c r="I24" s="41"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="33"/>
       <c r="B25" s="54" t="s">
         <v>84</v>
@@ -3655,7 +3668,7 @@
       <c r="I25" s="41"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="33"/>
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
@@ -3666,7 +3679,7 @@
       <c r="I26" s="41"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="33"/>
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
@@ -3681,7 +3694,7 @@
       <c r="I27" s="41"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="33"/>
       <c r="B28" s="54" t="s">
         <v>82</v>
@@ -3704,7 +3717,7 @@
       <c r="I28" s="41"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="33"/>
       <c r="B29" s="49"/>
       <c r="C29" s="49"/>
@@ -3715,7 +3728,7 @@
       <c r="I29" s="41"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="33"/>
       <c r="B30" s="49"/>
       <c r="C30" s="49"/>
@@ -3726,7 +3739,7 @@
       <c r="I30" s="41"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="33"/>
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
@@ -3737,7 +3750,7 @@
       <c r="I31" s="41"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
@@ -3793,12 +3806,12 @@
     </row>
     <row r="36" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="33"/>
-      <c r="B36" s="93" t="str">
+      <c r="B36" s="94" t="str">
         <f>CONCATENATE("Saldo na dzień ",ster!B3,ster!B2,":","                                                                                        [7]+[4]")</f>
         <v>Saldo na dzień 30.06.2024:                                                                                        [7]+[4]</v>
       </c>
-      <c r="C36" s="94"/>
-      <c r="D36" s="94"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
       <c r="E36" s="68"/>
       <c r="F36" s="81">
         <f>F33+F21</f>

</xml_diff>

<commit_message>
Add formal type of pdfs
</commit_message>
<xml_diff>
--- a/Woda062024.xlsx
+++ b/Woda062024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igi/Desktop/Projects/excelPDF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0AD221-3518-094A-A904-37BC900DD382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB81CF7-5004-5541-BB7F-A85078EC75E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{AD5EEB7A-8104-4FA8-A3F7-3232662F7F0C}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
   <si>
     <t>Rozliczenie lokali za wodę zimną i podgrzanie od 01.06.2024 do 30.06.2024</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t>wertex3233@gmail.com</t>
+  </si>
+  <si>
+    <t>adres kor</t>
+  </si>
+  <si>
+    <t>nabywca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiservice Sp. z o.o.|Stara Biała 1|09-411 Stara Biała </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MULTISERVICE Sp. z o.o.|Ul. Rynek 15-16|44-100 Gliwice|NIP:679-10-21-905 </t>
   </si>
 </sst>
 </file>
@@ -363,7 +375,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0000_ ;[Red]\-#,##0.0000\ "/>
     <numFmt numFmtId="167" formatCode="#,##0.000_ ;[Red]\-#,##0.000\ "/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +537,18 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="ArialMT"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -643,7 +667,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -927,6 +951,8 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1338,13 +1364,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79406D6C-E6C3-4E29-9900-755B942BAE09}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5:U28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" customWidth="1"/>
@@ -1352,7 +1378,7 @@
     <col min="23" max="23" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1409,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="14.5" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1410,7 +1436,7 @@
       <c r="T2" s="6"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" ht="70" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="70">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1474,8 +1500,14 @@
       <c r="U3" s="89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V3" t="s">
+        <v>91</v>
+      </c>
+      <c r="W3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
       <c r="C4" s="17">
@@ -1536,7 +1568,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="16">
       <c r="A5" s="87" t="s">
         <v>29</v>
       </c>
@@ -1600,8 +1632,14 @@
       <c r="U5" s="82" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="V5" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="W5" s="103" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="16">
       <c r="A6" s="87" t="s">
         <v>30</v>
       </c>
@@ -1665,8 +1703,9 @@
       <c r="U6" s="82" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="V6" s="104"/>
+    </row>
+    <row r="7" spans="1:23" ht="16">
       <c r="A7" s="87" t="s">
         <v>31</v>
       </c>
@@ -1731,7 +1770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="16">
       <c r="A8" s="87" t="s">
         <v>32</v>
       </c>
@@ -1796,7 +1835,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="16">
       <c r="A9" s="87" t="s">
         <v>33</v>
       </c>
@@ -1861,7 +1900,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="16">
       <c r="A10" s="87" t="s">
         <v>34</v>
       </c>
@@ -1926,7 +1965,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="16">
       <c r="A11" s="87" t="s">
         <v>35</v>
       </c>
@@ -1991,7 +2030,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="16">
       <c r="A12" s="87" t="s">
         <v>36</v>
       </c>
@@ -2056,7 +2095,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="16">
       <c r="A13" s="87" t="s">
         <v>37</v>
       </c>
@@ -2121,7 +2160,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="16">
       <c r="A14" s="87" t="s">
         <v>38</v>
       </c>
@@ -2186,7 +2225,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="16">
       <c r="A15" s="87" t="s">
         <v>39</v>
       </c>
@@ -2251,7 +2290,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="16">
       <c r="A16" s="87" t="s">
         <v>40</v>
       </c>
@@ -2288,7 +2327,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="16">
       <c r="A17" s="87" t="s">
         <v>41</v>
       </c>
@@ -2353,7 +2392,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="16">
       <c r="A18" s="87" t="s">
         <v>42</v>
       </c>
@@ -2418,7 +2457,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="16">
       <c r="A19" s="87" t="s">
         <v>36</v>
       </c>
@@ -2483,7 +2522,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="16">
       <c r="A20" s="87" t="s">
         <v>43</v>
       </c>
@@ -2548,7 +2587,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="16">
       <c r="A21" s="87" t="s">
         <v>44</v>
       </c>
@@ -2613,7 +2652,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="16">
       <c r="A22" s="87" t="s">
         <v>45</v>
       </c>
@@ -2678,7 +2717,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="16">
       <c r="A23" s="87" t="s">
         <v>46</v>
       </c>
@@ -2743,7 +2782,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="16">
       <c r="A24" s="87" t="s">
         <v>47</v>
       </c>
@@ -2808,7 +2847,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="16">
       <c r="A25" s="87" t="s">
         <v>48</v>
       </c>
@@ -2873,7 +2912,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="16">
       <c r="A26" s="87" t="s">
         <v>49</v>
       </c>
@@ -2938,7 +2977,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="16">
       <c r="A27" s="87" t="s">
         <v>50</v>
       </c>
@@ -3003,7 +3042,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="16">
       <c r="A28" s="88" t="s">
         <v>51</v>
       </c>
@@ -3068,7 +3107,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="6">
@@ -3123,7 +3162,7 @@
       </c>
       <c r="U29" s="24"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="6">
@@ -3176,7 +3215,7 @@
       </c>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="6">
@@ -3247,11 +3286,11 @@
   </sheetPr>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="107" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A15" zoomScale="107" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
@@ -3264,7 +3303,7 @@
     <col min="10" max="10" width="13.5" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="33"/>
       <c r="B1" s="33"/>
       <c r="C1" s="34"/>
@@ -3278,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="33"/>
       <c r="B2" s="96" t="s">
         <v>53</v>
@@ -3290,7 +3329,7 @@
       <c r="G2" s="96"/>
       <c r="H2" s="33"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="33"/>
       <c r="B3" s="33" t="s">
         <v>54</v>
@@ -3302,7 +3341,7 @@
       <c r="G3" s="33"/>
       <c r="H3" s="33"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="33"/>
       <c r="B4" s="33" t="s">
         <v>55</v>
@@ -3314,7 +3353,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="33"/>
       <c r="B5" s="37" t="s">
         <v>56</v>
@@ -3326,7 +3365,7 @@
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="33"/>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
@@ -3336,7 +3375,7 @@
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
     </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="19">
       <c r="A7" s="33"/>
       <c r="B7" s="97" t="s">
         <v>73</v>
@@ -3348,7 +3387,7 @@
       <c r="G7" s="97"/>
       <c r="H7" s="33"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="33"/>
       <c r="B8" s="33"/>
       <c r="C8" s="34"/>
@@ -3358,7 +3397,7 @@
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
     </row>
-    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="19">
       <c r="A9" s="33"/>
       <c r="B9" s="38" t="s">
         <v>57</v>
@@ -3373,7 +3412,7 @@
       <c r="G9" s="33"/>
       <c r="H9" s="33"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="33"/>
       <c r="B10" s="33" t="s">
         <v>58</v>
@@ -3388,7 +3427,7 @@
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="33"/>
       <c r="B11" s="33"/>
       <c r="C11" s="34"/>
@@ -3401,7 +3440,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="42.75" customHeight="1">
       <c r="A12" s="33"/>
       <c r="B12" s="98"/>
       <c r="C12" s="99"/>
@@ -3412,7 +3451,7 @@
       <c r="H12" s="33"/>
       <c r="J12" s="45"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="33"/>
       <c r="B13" s="33"/>
       <c r="C13" s="34"/>
@@ -3423,7 +3462,7 @@
       <c r="H13" s="33"/>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="16">
       <c r="A14" s="33"/>
       <c r="B14" s="100" t="s">
         <v>60</v>
@@ -3436,7 +3475,7 @@
       <c r="H14" s="33"/>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="33"/>
       <c r="B15" s="33"/>
       <c r="C15" s="46"/>
@@ -3447,7 +3486,7 @@
       <c r="H15" s="33"/>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="32">
       <c r="A16" s="33"/>
       <c r="B16" s="49" t="s">
         <v>80</v>
@@ -3467,7 +3506,7 @@
       <c r="I16" s="41"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="12.5" customHeight="1">
       <c r="A17" s="33"/>
       <c r="B17" s="48"/>
       <c r="C17" s="49"/>
@@ -3485,7 +3524,7 @@
       <c r="I17" s="41"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="33"/>
       <c r="B18" s="53" t="s">
         <v>75</v>
@@ -3522,7 +3561,7 @@
         <v>151.79</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="16">
       <c r="A19" s="33"/>
       <c r="B19" s="58" t="s">
         <v>76</v>
@@ -3547,7 +3586,7 @@
       <c r="I19" s="45"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="16">
       <c r="A20" s="33"/>
       <c r="B20" s="58" t="s">
         <v>79</v>
@@ -3569,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="16">
       <c r="A21" s="33"/>
       <c r="B21" s="50" t="s">
         <v>67</v>
@@ -3597,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="33"/>
       <c r="B22" s="33"/>
       <c r="C22" s="46"/>
@@ -3608,7 +3647,7 @@
       <c r="H22" s="33"/>
       <c r="J22" s="41"/>
     </row>
-    <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="32">
       <c r="A23" s="33"/>
       <c r="B23" s="49" t="s">
         <v>81</v>
@@ -3627,7 +3666,7 @@
       <c r="I23" s="41"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="12.5" customHeight="1">
       <c r="A24" s="33"/>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -3644,7 +3683,7 @@
       <c r="I24" s="41"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="12.5" customHeight="1">
       <c r="A25" s="33"/>
       <c r="B25" s="54" t="s">
         <v>84</v>
@@ -3668,7 +3707,7 @@
       <c r="I25" s="41"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="12.5" customHeight="1">
       <c r="A26" s="33"/>
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
@@ -3679,7 +3718,7 @@
       <c r="I26" s="41"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="12.5" customHeight="1">
       <c r="A27" s="33"/>
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
@@ -3694,7 +3733,7 @@
       <c r="I27" s="41"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="12.5" customHeight="1">
       <c r="A28" s="33"/>
       <c r="B28" s="54" t="s">
         <v>82</v>
@@ -3717,7 +3756,7 @@
       <c r="I28" s="41"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="12.5" customHeight="1">
       <c r="A29" s="33"/>
       <c r="B29" s="49"/>
       <c r="C29" s="49"/>
@@ -3728,7 +3767,7 @@
       <c r="I29" s="41"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="12.5" customHeight="1">
       <c r="A30" s="33"/>
       <c r="B30" s="49"/>
       <c r="C30" s="49"/>
@@ -3739,7 +3778,7 @@
       <c r="I30" s="41"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:13" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="12.5" customHeight="1">
       <c r="A31" s="33"/>
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
@@ -3750,7 +3789,7 @@
       <c r="I31" s="41"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="33"/>
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
@@ -3761,7 +3800,7 @@
       <c r="I32" s="41"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="17">
       <c r="A33" s="33"/>
       <c r="B33" s="63" t="s">
         <v>85</v>
@@ -3782,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="33"/>
       <c r="B34" s="33"/>
       <c r="C34" s="34"/>
@@ -3793,7 +3832,7 @@
       <c r="I34" s="41"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="33"/>
       <c r="B35" s="33"/>
       <c r="C35" s="34"/>
@@ -3804,7 +3843,7 @@
       <c r="H35" s="33"/>
       <c r="J35" s="41"/>
     </row>
-    <row r="36" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="63" customHeight="1">
       <c r="A36" s="33"/>
       <c r="B36" s="94" t="str">
         <f>CONCATENATE("Saldo na dzień ",ster!B3,ster!B2,":","                                                                                        [7]+[4]")</f>
@@ -3824,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="12.5" customHeight="1">
       <c r="A37" s="33"/>
       <c r="B37" s="33"/>
       <c r="C37" s="34"/>
@@ -3834,7 +3873,7 @@
       <c r="G37" s="33"/>
       <c r="H37" s="33"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="33"/>
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
@@ -3869,9 +3908,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -3879,7 +3918,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>52</v>
       </c>

</xml_diff>